<commit_message>
added more games, sped up simulate game logic, and drafted optimization logic
</commit_message>
<xml_diff>
--- a/team_specific_matrix/A&M-Corpus Christi_A.xlsx
+++ b/team_specific_matrix/A&M-Corpus Christi_A.xlsx
@@ -498,10 +498,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.2065217391304348</v>
+        <v>0.2202898550724638</v>
       </c>
       <c r="C2">
-        <v>0.5507246376811594</v>
+        <v>0.5130434782608696</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -522,7 +522,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.003623188405797101</v>
+        <v>0.01159420289855072</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.1413043478260869</v>
+        <v>0.1478260869565217</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -549,7 +549,7 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0.09782608695652174</v>
+        <v>0.1072463768115942</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -557,10 +557,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.0124223602484472</v>
+        <v>0.01063829787234043</v>
       </c>
       <c r="C3">
-        <v>0.02484472049689441</v>
+        <v>0.02659574468085106</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.07453416149068323</v>
+        <v>0.07446808510638298</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.7080745341614907</v>
+        <v>0.6968085106382979</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -608,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0.1801242236024845</v>
+        <v>0.1914893617021277</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -640,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.02777777777777778</v>
+        <v>0.02222222222222222</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -658,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.6388888888888888</v>
+        <v>0.7111111111111111</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0.3333333333333333</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -734,19 +734,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.07947019867549669</v>
+        <v>0.06598984771573604</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.01015228426395939</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.04635761589403974</v>
+        <v>0.05583756345177665</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -758,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.2582781456953642</v>
+        <v>0.2639593908629442</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -773,19 +773,19 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0.03311258278145696</v>
+        <v>0.03045685279187817</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>0.1390728476821192</v>
+        <v>0.1319796954314721</v>
       </c>
       <c r="R6">
-        <v>0.0728476821192053</v>
+        <v>0.08121827411167512</v>
       </c>
       <c r="S6">
-        <v>0.3708609271523179</v>
+        <v>0.3604060913705584</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -793,19 +793,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.125</v>
+        <v>0.1148936170212766</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.01630434782608696</v>
+        <v>0.01702127659574468</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.07065217391304347</v>
+        <v>0.05957446808510639</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.1576086956521739</v>
+        <v>0.1659574468085106</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -832,19 +832,19 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>0.01630434782608696</v>
+        <v>0.01276595744680851</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0.2010869565217391</v>
+        <v>0.1872340425531915</v>
       </c>
       <c r="R7">
-        <v>0.08152173913043478</v>
+        <v>0.07234042553191489</v>
       </c>
       <c r="S7">
-        <v>0.3315217391304348</v>
+        <v>0.3702127659574468</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -852,19 +852,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.08560311284046693</v>
+        <v>0.08554572271386431</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.03501945525291829</v>
+        <v>0.02949852507374631</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.03891050583657588</v>
+        <v>0.03244837758112094</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -876,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.1517509727626459</v>
+        <v>0.1651917404129793</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -891,19 +891,19 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>0.01167315175097276</v>
+        <v>0.01474926253687316</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0.1867704280155642</v>
+        <v>0.2035398230088496</v>
       </c>
       <c r="R8">
-        <v>0.0622568093385214</v>
+        <v>0.06194690265486726</v>
       </c>
       <c r="S8">
-        <v>0.4280155642023346</v>
+        <v>0.4070796460176991</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -911,7 +911,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.1166666666666667</v>
+        <v>0.12</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -923,7 +923,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.08333333333333333</v>
+        <v>0.08</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -935,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.1166666666666667</v>
+        <v>0.1066666666666667</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -950,19 +950,19 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>0.01666666666666667</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>0.2083333333333333</v>
+        <v>0.2133333333333333</v>
       </c>
       <c r="R9">
-        <v>0.04166666666666666</v>
+        <v>0.04666666666666667</v>
       </c>
       <c r="S9">
-        <v>0.4166666666666667</v>
+        <v>0.4066666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -970,19 +970,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.1393596986817326</v>
+        <v>0.1284403669724771</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.02448210922787194</v>
+        <v>0.0218772053634439</v>
       </c>
       <c r="E10">
-        <v>0.0009416195856873823</v>
+        <v>0.0007057163020465773</v>
       </c>
       <c r="F10">
-        <v>0.064030131826742</v>
+        <v>0.06563161609033169</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.1431261770244821</v>
+        <v>0.1446718419195483</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1009,19 +1009,19 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>0.01129943502824859</v>
+        <v>0.01199717713479181</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>0.211864406779661</v>
+        <v>0.2279463655610445</v>
       </c>
       <c r="R10">
-        <v>0.05367231638418079</v>
+        <v>0.05928016937191249</v>
       </c>
       <c r="S10">
-        <v>0.3512241054613936</v>
+        <v>0.3394495412844037</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -1044,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.1254612546125461</v>
+        <v>0.1324324324324324</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1053,13 +1053,13 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0.07749077490774908</v>
+        <v>0.0918918918918919</v>
       </c>
       <c r="K11">
-        <v>0.1512915129151292</v>
+        <v>0.1756756756756757</v>
       </c>
       <c r="L11">
-        <v>0.6346863468634686</v>
+        <v>0.5837837837837838</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1080,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>0.01107011070110701</v>
+        <v>0.01621621621621622</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1103,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.6927374301675978</v>
+        <v>0.7104072398190046</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1112,13 +1112,13 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0.2625698324022346</v>
+        <v>0.253393665158371</v>
       </c>
       <c r="K12">
-        <v>0.01675977653631285</v>
+        <v>0.01357466063348416</v>
       </c>
       <c r="L12">
-        <v>0.0111731843575419</v>
+        <v>0.009049773755656109</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>0.01675977653631285</v>
+        <v>0.01357466063348416</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1159,10 +1159,10 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0.02272727272727273</v>
+        <v>0.02</v>
       </c>
       <c r="G13">
-        <v>0.6818181818181818</v>
+        <v>0.72</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0.2727272727272727</v>
+        <v>0.24</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1198,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>0.02272727272727273</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1277,34 +1277,34 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0.006097560975609756</v>
+        <v>0.004629629629629629</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.1402439024390244</v>
+        <v>0.125</v>
       </c>
       <c r="I15">
-        <v>0.07317073170731707</v>
+        <v>0.06944444444444445</v>
       </c>
       <c r="J15">
-        <v>0.4634146341463415</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="K15">
-        <v>0.05487804878048781</v>
+        <v>0.06018518518518518</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0.02439024390243903</v>
+        <v>0.02314814814814815</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15">
-        <v>0.0426829268292683</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -1316,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>0.1951219512195122</v>
+        <v>0.2175925925925926</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -1336,34 +1336,34 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0.02352941176470588</v>
+        <v>0.01932367149758454</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0.1529411764705882</v>
+        <v>0.1352657004830918</v>
       </c>
       <c r="I16">
-        <v>0.05882352941176471</v>
+        <v>0.05314009661835749</v>
       </c>
       <c r="J16">
-        <v>0.4823529411764706</v>
+        <v>0.4975845410628019</v>
       </c>
       <c r="K16">
-        <v>0.1352941176470588</v>
+        <v>0.1400966183574879</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0.01764705882352941</v>
+        <v>0.01932367149758454</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16">
-        <v>0.04117647058823529</v>
+        <v>0.04830917874396135</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -1375,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="S16">
-        <v>0.08823529411764706</v>
+        <v>0.08695652173913043</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -1395,34 +1395,34 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0.01392757660167131</v>
+        <v>0.01814516129032258</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0.1532033426183844</v>
+        <v>0.1391129032258064</v>
       </c>
       <c r="I17">
-        <v>0.06685236768802229</v>
+        <v>0.07459677419354839</v>
       </c>
       <c r="J17">
-        <v>0.4540389972144847</v>
+        <v>0.4596774193548387</v>
       </c>
       <c r="K17">
-        <v>0.1309192200557103</v>
+        <v>0.1290322580645161</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>0.02785515320334262</v>
+        <v>0.02016129032258064</v>
       </c>
       <c r="N17">
-        <v>0.005571030640668524</v>
+        <v>0.004032258064516129</v>
       </c>
       <c r="O17">
-        <v>0.07242339832869081</v>
+        <v>0.07056451612903226</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -1434,7 +1434,7 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>0.07520891364902507</v>
+        <v>0.0846774193548387</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -1454,34 +1454,34 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0.009708737864077669</v>
+        <v>0.006944444444444444</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0.1359223300970874</v>
+        <v>0.1597222222222222</v>
       </c>
       <c r="I18">
-        <v>0.05825242718446602</v>
+        <v>0.04861111111111111</v>
       </c>
       <c r="J18">
-        <v>0.3980582524271845</v>
+        <v>0.4375</v>
       </c>
       <c r="K18">
-        <v>0.1941747572815534</v>
+        <v>0.1736111111111111</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>0.02912621359223301</v>
+        <v>0.02777777777777778</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18">
-        <v>0.06796116504854369</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>0.1067961165048544</v>
+        <v>0.09027777777777778</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -1513,34 +1513,34 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0.01565995525727069</v>
+        <v>0.01558441558441558</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0.1554809843400447</v>
+        <v>0.1662337662337662</v>
       </c>
       <c r="I19">
-        <v>0.07718120805369127</v>
+        <v>0.07012987012987013</v>
       </c>
       <c r="J19">
-        <v>0.3914988814317674</v>
+        <v>0.3939393939393939</v>
       </c>
       <c r="K19">
-        <v>0.1409395973154362</v>
+        <v>0.1454545454545454</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>0.029082774049217</v>
+        <v>0.02510822510822511</v>
       </c>
       <c r="N19">
         <v>0</v>
       </c>
       <c r="O19">
-        <v>0.08165548098434004</v>
+        <v>0.08051948051948052</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -1552,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="S19">
-        <v>0.1085011185682327</v>
+        <v>0.103030303030303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to team matrices from games pulled march 7
</commit_message>
<xml_diff>
--- a/team_specific_matrix/A&M-Corpus Christi_A.xlsx
+++ b/team_specific_matrix/A&M-Corpus Christi_A.xlsx
@@ -498,10 +498,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.2172774869109948</v>
+        <v>0.2125</v>
       </c>
       <c r="C2">
-        <v>0.5209424083769634</v>
+        <v>0.5275</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -522,7 +522,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.01308900523560209</v>
+        <v>0.015</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.1465968586387434</v>
+        <v>0.145</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -549,7 +549,7 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0.1020942408376963</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -557,10 +557,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.009523809523809525</v>
+        <v>0.008968609865470852</v>
       </c>
       <c r="C3">
-        <v>0.02380952380952381</v>
+        <v>0.02242152466367713</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.07142857142857142</v>
+        <v>0.07174887892376682</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.719047619047619</v>
+        <v>0.7174887892376681</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -608,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0.1761904761904762</v>
+        <v>0.179372197309417</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -640,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.02</v>
+        <v>0.0196078431372549</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -658,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.74</v>
+        <v>0.7450980392156863</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0.24</v>
+        <v>0.2352941176470588</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -734,19 +734,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.06018518518518518</v>
+        <v>0.05957446808510639</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.009259259259259259</v>
+        <v>0.008510638297872341</v>
       </c>
       <c r="E6">
-        <v>0.004629629629629629</v>
+        <v>0.00425531914893617</v>
       </c>
       <c r="F6">
-        <v>0.05092592592592592</v>
+        <v>0.05106382978723404</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -758,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.2592592592592592</v>
+        <v>0.2553191489361702</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -773,19 +773,19 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0.03240740740740741</v>
+        <v>0.03404255319148936</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>0.1527777777777778</v>
+        <v>0.148936170212766</v>
       </c>
       <c r="R6">
-        <v>0.07407407407407407</v>
+        <v>0.07659574468085106</v>
       </c>
       <c r="S6">
-        <v>0.3564814814814815</v>
+        <v>0.3617021276595745</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -793,19 +793,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.1167315175097276</v>
+        <v>0.1163636363636364</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.01945525291828794</v>
+        <v>0.01818181818181818</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.05836575875486381</v>
+        <v>0.05818181818181818</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.1673151750972763</v>
+        <v>0.1672727272727273</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -832,19 +832,19 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>0.01945525291828794</v>
+        <v>0.01818181818181818</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0.1867704280155642</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="R7">
-        <v>0.07003891050583658</v>
+        <v>0.06545454545454546</v>
       </c>
       <c r="S7">
-        <v>0.3618677042801556</v>
+        <v>0.3745454545454546</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -852,19 +852,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.09183673469387756</v>
+        <v>0.09156626506024096</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.02551020408163265</v>
+        <v>0.02409638554216868</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.03316326530612245</v>
+        <v>0.03132530120481928</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -876,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.1581632653061225</v>
+        <v>0.1542168674698795</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -891,19 +891,19 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>0.01275510204081633</v>
+        <v>0.01445783132530121</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0.2219387755102041</v>
+        <v>0.2289156626506024</v>
       </c>
       <c r="R8">
-        <v>0.06377551020408163</v>
+        <v>0.06024096385542169</v>
       </c>
       <c r="S8">
-        <v>0.3928571428571428</v>
+        <v>0.3951807228915662</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -911,7 +911,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.1265060240963855</v>
+        <v>0.125</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -923,7 +923,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.0783132530120482</v>
+        <v>0.07954545454545454</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -935,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.0963855421686747</v>
+        <v>0.1022727272727273</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -950,19 +950,19 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>0.03012048192771084</v>
+        <v>0.02840909090909091</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>0.2108433734939759</v>
+        <v>0.2159090909090909</v>
       </c>
       <c r="R9">
-        <v>0.04216867469879518</v>
+        <v>0.03977272727272727</v>
       </c>
       <c r="S9">
-        <v>0.4156626506024096</v>
+        <v>0.4090909090909091</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -970,19 +970,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.1269230769230769</v>
+        <v>0.1243275552898984</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.02243589743589744</v>
+        <v>0.02151823072325165</v>
       </c>
       <c r="E10">
-        <v>0.000641025641025641</v>
+        <v>0.0005977286312014345</v>
       </c>
       <c r="F10">
-        <v>0.06602564102564103</v>
+        <v>0.06814106395696354</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.1403846153846154</v>
+        <v>0.1410639569635385</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1009,19 +1009,19 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>0.01153846153846154</v>
+        <v>0.01195457262402869</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>0.2307692307692308</v>
+        <v>0.2331141661685595</v>
       </c>
       <c r="R10">
-        <v>0.05961538461538462</v>
+        <v>0.05977286312014345</v>
       </c>
       <c r="S10">
-        <v>0.3416666666666667</v>
+        <v>0.3395098625224148</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -1044,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.1418269230769231</v>
+        <v>0.1460674157303371</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1053,13 +1053,13 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0.09134615384615384</v>
+        <v>0.0898876404494382</v>
       </c>
       <c r="K11">
-        <v>0.1826923076923077</v>
+        <v>0.1887640449438202</v>
       </c>
       <c r="L11">
-        <v>0.5673076923076923</v>
+        <v>0.5595505617977528</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1080,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>0.01682692307692308</v>
+        <v>0.01573033707865169</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1103,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.6916666666666667</v>
+        <v>0.7023809523809523</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1112,13 +1112,13 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0.2708333333333333</v>
+        <v>0.2619047619047619</v>
       </c>
       <c r="K12">
-        <v>0.01666666666666667</v>
+        <v>0.01587301587301587</v>
       </c>
       <c r="L12">
-        <v>0.008333333333333333</v>
+        <v>0.007936507936507936</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>0.0125</v>
+        <v>0.0119047619047619</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1221,7 +1221,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0.5</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1230,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0.5</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1277,34 +1277,34 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0.01214574898785425</v>
+        <v>0.01503759398496241</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.1336032388663968</v>
+        <v>0.1240601503759398</v>
       </c>
       <c r="I15">
-        <v>0.06882591093117409</v>
+        <v>0.06766917293233082</v>
       </c>
       <c r="J15">
-        <v>0.4412955465587045</v>
+        <v>0.443609022556391</v>
       </c>
       <c r="K15">
-        <v>0.06072874493927125</v>
+        <v>0.05639097744360902</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0.02024291497975709</v>
+        <v>0.01879699248120301</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15">
-        <v>0.048582995951417</v>
+        <v>0.05263157894736842</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -1316,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>0.2145748987854251</v>
+        <v>0.2218045112781955</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -1336,34 +1336,34 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0.01694915254237288</v>
+        <v>0.01612903225806452</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0.1440677966101695</v>
+        <v>0.1451612903225807</v>
       </c>
       <c r="I16">
-        <v>0.05932203389830509</v>
+        <v>0.06048387096774194</v>
       </c>
       <c r="J16">
-        <v>0.4915254237288136</v>
+        <v>0.4919354838709677</v>
       </c>
       <c r="K16">
-        <v>0.1355932203389831</v>
+        <v>0.1290322580645161</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0.0211864406779661</v>
+        <v>0.02016129032258064</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16">
-        <v>0.05084745762711865</v>
+        <v>0.05241935483870968</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -1375,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="S16">
-        <v>0.08050847457627118</v>
+        <v>0.0846774193548387</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -1395,34 +1395,34 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0.01773049645390071</v>
+        <v>0.01642036124794746</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0.1436170212765958</v>
+        <v>0.1412151067323481</v>
       </c>
       <c r="I17">
-        <v>0.07624113475177305</v>
+        <v>0.07060755336617405</v>
       </c>
       <c r="J17">
-        <v>0.4556737588652482</v>
+        <v>0.4696223316912972</v>
       </c>
       <c r="K17">
-        <v>0.1294326241134752</v>
+        <v>0.1280788177339902</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>0.01773049645390071</v>
+        <v>0.01642036124794746</v>
       </c>
       <c r="N17">
-        <v>0.003546099290780142</v>
+        <v>0.004926108374384237</v>
       </c>
       <c r="O17">
-        <v>0.06560283687943262</v>
+        <v>0.06075533661740559</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -1434,7 +1434,7 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>0.09042553191489362</v>
+        <v>0.09195402298850575</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -1454,34 +1454,34 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0.006329113924050633</v>
+        <v>0.005988023952095809</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0.1518987341772152</v>
+        <v>0.1497005988023952</v>
       </c>
       <c r="I18">
-        <v>0.05063291139240506</v>
+        <v>0.04790419161676647</v>
       </c>
       <c r="J18">
-        <v>0.4430379746835443</v>
+        <v>0.437125748502994</v>
       </c>
       <c r="K18">
-        <v>0.1582278481012658</v>
+        <v>0.155688622754491</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>0.03164556962025317</v>
+        <v>0.02994011976047904</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18">
-        <v>0.06329113924050633</v>
+        <v>0.0718562874251497</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>0.0949367088607595</v>
+        <v>0.1017964071856287</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -1513,34 +1513,34 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0.01410658307210031</v>
+        <v>0.01457725947521866</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0.1724137931034483</v>
+        <v>0.1712827988338192</v>
       </c>
       <c r="I19">
-        <v>0.06661442006269593</v>
+        <v>0.06778425655976676</v>
       </c>
       <c r="J19">
-        <v>0.3894984326018809</v>
+        <v>0.3870262390670554</v>
       </c>
       <c r="K19">
-        <v>0.1473354231974922</v>
+        <v>0.1479591836734694</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>0.02351097178683386</v>
+        <v>0.02259475218658892</v>
       </c>
       <c r="N19">
         <v>0</v>
       </c>
       <c r="O19">
-        <v>0.08307210031347963</v>
+        <v>0.08309037900874636</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -1552,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="S19">
-        <v>0.103448275862069</v>
+        <v>0.1056851311953353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>